<commit_message>
format changes in notebook and write up
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arnab Learning\AI_ML_DS\EPGP_IIITB_Upgrad\Course 7 - Course 4 - Deep Learning\Module 7 - Gesture Recognition Project\Git_Repo\Gesture-Recognition-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64A77700-286F-4EAB-8281-14435F6C7735}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AD6B1C-A2BB-457E-8DE5-7C8B91EC88AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{5F067AC9-599E-4E59-A365-A6D113994EE3}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5F067AC9-599E-4E59-A365-A6D113994EE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -619,7 +619,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -627,9 +627,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -640,9 +637,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="1" fillId="5" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -660,9 +654,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -678,16 +669,10 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -696,7 +681,7 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
@@ -707,6 +692,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1025,8 +1016,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80923883-5B62-4AF5-AE7C-62BC6F87EDBB}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="A19" sqref="A19:O24"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
@@ -1036,1090 +1027,1090 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:15" ht="62.5" thickBot="1">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C1" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E1" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I1" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J1" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K1" s="8" t="s">
+      <c r="K1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="L1" s="7" t="s">
+      <c r="L1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="M1" s="8" t="s">
+      <c r="M1" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="N1" s="7" t="s">
+      <c r="N1" s="6" t="s">
         <v>114</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="O1" s="8" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="160.5" thickTop="1" thickBot="1">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="B2" s="11">
+      <c r="B2" s="9">
         <v>1</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E2" s="9">
         <v>15</v>
       </c>
-      <c r="F2" s="11" t="s">
+      <c r="F2" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G2" s="11">
+      <c r="G2" s="9">
         <v>1E-3</v>
       </c>
-      <c r="H2" s="11">
+      <c r="H2" s="9">
         <v>50</v>
       </c>
-      <c r="I2" s="11">
+      <c r="I2" s="9">
         <v>32</v>
       </c>
-      <c r="J2" s="17">
+      <c r="J2" s="14">
         <v>0.8125</v>
       </c>
-      <c r="K2" s="18">
+      <c r="K2" s="15">
         <v>0.608326435089111</v>
       </c>
-      <c r="L2" s="17">
+      <c r="L2" s="14">
         <v>0.92090000000000005</v>
       </c>
-      <c r="M2" s="18">
+      <c r="M2" s="15">
         <v>0.43059999999999998</v>
       </c>
-      <c r="N2" s="11">
+      <c r="N2" s="9">
         <v>36</v>
       </c>
-      <c r="O2" s="12" t="s">
+      <c r="O2" s="10" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="3" spans="1:15" ht="160.5" thickTop="1" thickBot="1">
-      <c r="A3" s="10"/>
-      <c r="B3" s="13">
+      <c r="A3" s="27"/>
+      <c r="B3" s="11">
         <v>2</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D3" s="14" t="s">
+      <c r="D3" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E3" s="13">
+      <c r="E3" s="11">
         <v>15</v>
       </c>
-      <c r="F3" s="13" t="s">
+      <c r="F3" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G3" s="13">
+      <c r="G3" s="11">
         <v>1E-3</v>
       </c>
-      <c r="H3" s="13">
+      <c r="H3" s="11">
         <v>50</v>
       </c>
-      <c r="I3" s="13">
+      <c r="I3" s="11">
         <v>32</v>
       </c>
-      <c r="J3" s="19">
+      <c r="J3" s="16">
         <v>0.875</v>
       </c>
-      <c r="K3" s="20">
+      <c r="K3" s="17">
         <v>0.61729753017425504</v>
       </c>
-      <c r="L3" s="19">
+      <c r="L3" s="16">
         <v>0.71699999999999997</v>
       </c>
-      <c r="M3" s="20">
+      <c r="M3" s="17">
         <v>0.7581</v>
       </c>
-      <c r="N3" s="13">
+      <c r="N3" s="11">
         <v>40</v>
       </c>
-      <c r="O3" s="15" t="s">
+      <c r="O3" s="13" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="4" spans="1:15" ht="160.5" thickTop="1" thickBot="1">
-      <c r="A4" s="10"/>
-      <c r="B4" s="11">
+      <c r="A4" s="27"/>
+      <c r="B4" s="9">
         <v>3</v>
       </c>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="E4" s="11">
+      <c r="E4" s="9">
         <v>15</v>
       </c>
-      <c r="F4" s="11" t="s">
+      <c r="F4" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G4" s="11">
+      <c r="G4" s="9">
         <v>1E-3</v>
       </c>
-      <c r="H4" s="11">
+      <c r="H4" s="9">
         <v>50</v>
       </c>
-      <c r="I4" s="11">
+      <c r="I4" s="9">
         <v>32</v>
       </c>
-      <c r="J4" s="17">
+      <c r="J4" s="14">
         <v>0.9375</v>
       </c>
-      <c r="K4" s="18">
+      <c r="K4" s="15">
         <v>0.562585949897766</v>
       </c>
-      <c r="L4" s="17">
+      <c r="L4" s="14">
         <v>0.6744</v>
       </c>
-      <c r="M4" s="18">
+      <c r="M4" s="15">
         <v>0.85199999999999998</v>
       </c>
-      <c r="N4" s="11">
+      <c r="N4" s="9">
         <v>38</v>
       </c>
-      <c r="O4" s="12" t="s">
+      <c r="O4" s="10" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="160.5" thickTop="1" thickBot="1">
-      <c r="A5" s="10"/>
-      <c r="B5" s="13">
+      <c r="A5" s="27"/>
+      <c r="B5" s="11">
         <v>4</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="13" t="s">
+      <c r="D5" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E5" s="14">
+      <c r="E5" s="12">
         <v>20</v>
       </c>
-      <c r="F5" s="13" t="s">
+      <c r="F5" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G5" s="13">
+      <c r="G5" s="11">
         <v>1E-3</v>
       </c>
-      <c r="H5" s="13">
+      <c r="H5" s="11">
         <v>50</v>
       </c>
-      <c r="I5" s="13">
+      <c r="I5" s="11">
         <v>32</v>
       </c>
-      <c r="J5" s="19">
+      <c r="J5" s="16">
         <v>0.875</v>
       </c>
-      <c r="K5" s="20">
+      <c r="K5" s="17">
         <v>0.43138277530670099</v>
       </c>
-      <c r="L5" s="19">
+      <c r="L5" s="16">
         <v>0.86450000000000005</v>
       </c>
-      <c r="M5" s="20">
+      <c r="M5" s="17">
         <v>0.46260000000000001</v>
       </c>
-      <c r="N5" s="13">
+      <c r="N5" s="11">
         <v>40</v>
       </c>
-      <c r="O5" s="15" t="s">
+      <c r="O5" s="13" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="160.5" thickTop="1" thickBot="1">
-      <c r="A6" s="10"/>
-      <c r="B6" s="11">
+      <c r="A6" s="27"/>
+      <c r="B6" s="9">
         <v>5</v>
       </c>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="E6" s="11">
+      <c r="E6" s="9">
         <v>20</v>
       </c>
-      <c r="F6" s="11" t="s">
+      <c r="F6" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G6" s="11">
+      <c r="G6" s="9">
         <v>1E-3</v>
       </c>
-      <c r="H6" s="11">
+      <c r="H6" s="9">
         <v>50</v>
       </c>
-      <c r="I6" s="11">
+      <c r="I6" s="9">
         <v>32</v>
       </c>
-      <c r="J6" s="17">
+      <c r="J6" s="14">
         <v>0.8125</v>
       </c>
-      <c r="K6" s="18">
+      <c r="K6" s="15">
         <v>0.91410553455352705</v>
       </c>
-      <c r="L6" s="17">
+      <c r="L6" s="14">
         <v>0.60780000000000001</v>
       </c>
-      <c r="M6" s="18">
+      <c r="M6" s="15">
         <v>1.0878000000000001</v>
       </c>
-      <c r="N6" s="11">
+      <c r="N6" s="9">
         <v>40</v>
       </c>
-      <c r="O6" s="12" t="s">
+      <c r="O6" s="10" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="146" thickTop="1" thickBot="1">
-      <c r="A7" s="10"/>
-      <c r="B7" s="13">
+      <c r="A7" s="27"/>
+      <c r="B7" s="11">
         <v>6</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D7" s="14" t="s">
+      <c r="D7" s="12" t="s">
         <v>77</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="11">
         <v>20</v>
       </c>
-      <c r="F7" s="13" t="s">
+      <c r="F7" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G7" s="13">
+      <c r="G7" s="11">
         <v>1E-3</v>
       </c>
-      <c r="H7" s="13">
+      <c r="H7" s="11">
         <v>50</v>
       </c>
-      <c r="I7" s="13">
+      <c r="I7" s="11">
         <v>32</v>
       </c>
-      <c r="J7" s="19">
+      <c r="J7" s="16">
         <v>1</v>
       </c>
-      <c r="K7" s="20">
+      <c r="K7" s="17">
         <v>0.72884345054626398</v>
       </c>
-      <c r="L7" s="19">
+      <c r="L7" s="16">
         <v>0.72160000000000002</v>
       </c>
-      <c r="M7" s="20">
+      <c r="M7" s="17">
         <v>0.86639999999999995</v>
       </c>
-      <c r="N7" s="13">
+      <c r="N7" s="11">
         <v>49</v>
       </c>
-      <c r="O7" s="15" t="s">
+      <c r="O7" s="13" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="146" thickTop="1" thickBot="1">
-      <c r="A8" s="10"/>
-      <c r="B8" s="11">
+      <c r="A8" s="27"/>
+      <c r="B8" s="9">
         <v>7</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="C8" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D8" s="14" t="s">
+      <c r="D8" s="12" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="11">
+      <c r="E8" s="9">
         <v>20</v>
       </c>
-      <c r="F8" s="11" t="s">
+      <c r="F8" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="11">
+      <c r="G8" s="9">
         <v>1E-3</v>
       </c>
-      <c r="H8" s="11">
+      <c r="H8" s="9">
         <v>50</v>
       </c>
-      <c r="I8" s="11">
+      <c r="I8" s="9">
         <v>32</v>
       </c>
-      <c r="J8" s="17">
+      <c r="J8" s="14">
         <v>1</v>
       </c>
-      <c r="K8" s="18">
+      <c r="K8" s="15">
         <v>0.72884345054626398</v>
       </c>
-      <c r="L8" s="17">
+      <c r="L8" s="14">
         <v>0.70868349075317305</v>
       </c>
-      <c r="M8" s="18">
+      <c r="M8" s="15">
         <v>0.82833945751190097</v>
       </c>
-      <c r="N8" s="11">
+      <c r="N8" s="9">
         <v>50</v>
       </c>
-      <c r="O8" s="12" t="s">
+      <c r="O8" s="10" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="146" thickTop="1" thickBot="1">
-      <c r="A9" s="10"/>
-      <c r="B9" s="13">
+      <c r="A9" s="27"/>
+      <c r="B9" s="11">
         <v>8</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="11">
         <v>20</v>
       </c>
-      <c r="F9" s="13" t="s">
+      <c r="F9" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G9" s="13">
+      <c r="G9" s="11">
         <v>1E-3</v>
       </c>
-      <c r="H9" s="13">
+      <c r="H9" s="11">
         <v>50</v>
       </c>
-      <c r="I9" s="13">
+      <c r="I9" s="11">
         <v>32</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="16">
         <v>0.9375</v>
       </c>
-      <c r="K9" s="20">
+      <c r="K9" s="17">
         <v>0.45960000000000001</v>
       </c>
-      <c r="L9" s="19">
+      <c r="L9" s="16">
         <v>0.83340000000000003</v>
       </c>
-      <c r="M9" s="20">
+      <c r="M9" s="17">
         <v>0.58689999999999998</v>
       </c>
-      <c r="N9" s="13">
+      <c r="N9" s="11">
         <v>49</v>
       </c>
-      <c r="O9" s="15" t="s">
+      <c r="O9" s="13" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:15" ht="146" thickTop="1" thickBot="1">
-      <c r="A10" s="10"/>
-      <c r="B10" s="16">
+      <c r="A10" s="27"/>
+      <c r="B10" s="9">
         <v>9</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="C10" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="E10" s="11">
+      <c r="E10" s="9">
         <v>20</v>
       </c>
-      <c r="F10" s="14" t="s">
+      <c r="F10" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="11">
+      <c r="G10" s="9">
         <v>1E-3</v>
       </c>
-      <c r="H10" s="11">
+      <c r="H10" s="9">
         <v>50</v>
       </c>
-      <c r="I10" s="11">
+      <c r="I10" s="9">
         <v>32</v>
       </c>
-      <c r="J10" s="21">
+      <c r="J10" s="18">
         <v>0.875</v>
       </c>
-      <c r="K10" s="22">
+      <c r="K10" s="15">
         <v>0.33637839555740301</v>
       </c>
-      <c r="L10" s="21">
+      <c r="L10" s="18">
         <v>0.8861</v>
       </c>
-      <c r="M10" s="22">
+      <c r="M10" s="15">
         <v>0.45900000000000002</v>
       </c>
-      <c r="N10" s="16">
+      <c r="N10" s="9">
         <v>53</v>
       </c>
-      <c r="O10" s="12" t="s">
+      <c r="O10" s="10" t="s">
         <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:15" ht="146" thickTop="1" thickBot="1">
-      <c r="A11" s="10"/>
-      <c r="B11" s="13">
+      <c r="A11" s="27"/>
+      <c r="B11" s="11">
         <v>10</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D11" s="14" t="s">
+      <c r="D11" s="12" t="s">
         <v>79</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E11" s="11">
         <v>20</v>
       </c>
-      <c r="F11" s="13" t="s">
+      <c r="F11" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="13">
+      <c r="G11" s="11">
         <v>1E-3</v>
       </c>
-      <c r="H11" s="13">
+      <c r="H11" s="11">
         <v>50</v>
       </c>
-      <c r="I11" s="13">
+      <c r="I11" s="11">
         <v>32</v>
       </c>
-      <c r="J11" s="19">
+      <c r="J11" s="16">
         <v>0.875</v>
       </c>
-      <c r="K11" s="20">
+      <c r="K11" s="17">
         <v>0.34926694631576499</v>
       </c>
-      <c r="L11" s="19">
+      <c r="L11" s="16">
         <v>0.73329999999999995</v>
       </c>
-      <c r="M11" s="20">
+      <c r="M11" s="17">
         <v>0.71120000000000005</v>
       </c>
-      <c r="N11" s="13">
+      <c r="N11" s="11">
         <v>52</v>
       </c>
-      <c r="O11" s="15" t="s">
+      <c r="O11" s="13" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="12" spans="1:15" ht="146" thickTop="1" thickBot="1">
-      <c r="A12" s="10"/>
-      <c r="B12" s="16">
+      <c r="A12" s="27"/>
+      <c r="B12" s="9">
         <v>11</v>
       </c>
-      <c r="C12" s="16" t="s">
+      <c r="C12" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="E12" s="11">
+      <c r="E12" s="9">
         <v>20</v>
       </c>
-      <c r="F12" s="14" t="s">
+      <c r="F12" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G12" s="11">
+      <c r="G12" s="9">
         <v>1E-3</v>
       </c>
-      <c r="H12" s="11">
+      <c r="H12" s="9">
         <v>50</v>
       </c>
-      <c r="I12" s="11">
+      <c r="I12" s="9">
         <v>32</v>
       </c>
-      <c r="J12" s="17">
+      <c r="J12" s="14">
         <v>0.875</v>
       </c>
-      <c r="K12" s="22">
+      <c r="K12" s="15">
         <v>0.34926694631576499</v>
       </c>
-      <c r="L12" s="21">
+      <c r="L12" s="18">
         <v>0.77591037750244096</v>
       </c>
-      <c r="M12" s="22">
+      <c r="M12" s="15">
         <v>0.71120000000000005</v>
       </c>
-      <c r="N12" s="16">
+      <c r="N12" s="9">
         <v>51</v>
       </c>
-      <c r="O12" s="12" t="s">
+      <c r="O12" s="10" t="s">
         <v>93</v>
       </c>
     </row>
     <row r="13" spans="1:15" ht="146" thickTop="1" thickBot="1">
-      <c r="A13" s="10"/>
-      <c r="B13" s="13">
+      <c r="A13" s="27"/>
+      <c r="B13" s="11">
         <v>12</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="13" t="s">
+      <c r="D13" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="11">
         <v>20</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="12" t="s">
         <v>81</v>
       </c>
-      <c r="H13" s="13">
+      <c r="H13" s="11">
         <v>50</v>
       </c>
-      <c r="I13" s="13">
+      <c r="I13" s="11">
         <v>32</v>
       </c>
-      <c r="J13" s="19">
+      <c r="J13" s="16">
         <v>0.8125</v>
       </c>
-      <c r="K13" s="20">
+      <c r="K13" s="17">
         <v>0.491327404975891</v>
       </c>
-      <c r="L13" s="19">
+      <c r="L13" s="16">
         <v>0.62190000000000001</v>
       </c>
-      <c r="M13" s="20">
+      <c r="M13" s="17">
         <v>0.94269999999999998</v>
       </c>
-      <c r="N13" s="13">
+      <c r="N13" s="11">
         <v>50</v>
       </c>
-      <c r="O13" s="15" t="s">
+      <c r="O13" s="13" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="14" spans="1:15" ht="189.5" thickTop="1" thickBot="1">
-      <c r="A14" s="10" t="s">
+      <c r="A14" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="B14" s="11">
+      <c r="B14" s="9">
         <v>1</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D14" s="14" t="s">
+      <c r="D14" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="E14" s="11">
+      <c r="E14" s="9">
         <v>20</v>
       </c>
-      <c r="F14" s="14" t="s">
+      <c r="F14" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="G14" s="11">
+      <c r="G14" s="9">
         <v>1E-3</v>
       </c>
-      <c r="H14" s="11">
+      <c r="H14" s="9">
         <v>50</v>
       </c>
-      <c r="I14" s="11">
+      <c r="I14" s="9">
         <v>32</v>
       </c>
-      <c r="J14" s="17">
+      <c r="J14" s="14">
         <v>0.75</v>
       </c>
-      <c r="K14" s="18">
+      <c r="K14" s="15">
         <v>1.0346825122833201</v>
       </c>
-      <c r="L14" s="17">
+      <c r="L14" s="14">
         <v>0.438</v>
       </c>
-      <c r="M14" s="18">
+      <c r="M14" s="15">
         <v>1.3465</v>
       </c>
-      <c r="N14" s="11">
+      <c r="N14" s="9">
         <v>61</v>
       </c>
-      <c r="O14" s="29" t="s">
+      <c r="O14" s="24" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="189.5" thickTop="1" thickBot="1">
-      <c r="A15" s="10"/>
-      <c r="B15" s="13">
+      <c r="A15" s="27"/>
+      <c r="B15" s="11">
         <v>2</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D15" s="14" t="s">
+      <c r="D15" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="E15" s="13">
+      <c r="E15" s="11">
         <v>20</v>
       </c>
-      <c r="F15" s="13" t="s">
+      <c r="F15" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="G15" s="13">
+      <c r="G15" s="11">
         <v>1E-3</v>
       </c>
-      <c r="H15" s="13">
+      <c r="H15" s="11">
         <v>50</v>
       </c>
-      <c r="I15" s="13">
+      <c r="I15" s="11">
         <v>32</v>
       </c>
-      <c r="J15" s="19">
+      <c r="J15" s="16">
         <v>0.6875</v>
       </c>
-      <c r="K15" s="20">
+      <c r="K15" s="17">
         <v>0.88131904602050704</v>
       </c>
-      <c r="L15" s="19">
+      <c r="L15" s="16">
         <v>0.60040000000000004</v>
       </c>
-      <c r="M15" s="20">
+      <c r="M15" s="17">
         <v>1.0636000000000001</v>
       </c>
-      <c r="N15" s="13">
+      <c r="N15" s="11">
         <v>61</v>
       </c>
-      <c r="O15" s="29" t="s">
+      <c r="O15" s="24" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="16" spans="1:15" ht="189.5" thickTop="1" thickBot="1">
-      <c r="A16" s="10"/>
-      <c r="B16" s="16">
+      <c r="A16" s="27"/>
+      <c r="B16" s="9">
         <v>3</v>
       </c>
-      <c r="C16" s="16" t="s">
+      <c r="C16" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D16" s="14" t="s">
+      <c r="D16" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="E16" s="16">
+      <c r="E16" s="9">
         <v>20</v>
       </c>
-      <c r="F16" s="16" t="s">
+      <c r="F16" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G16" s="16">
+      <c r="G16" s="9">
         <v>1E-3</v>
       </c>
-      <c r="H16" s="16">
+      <c r="H16" s="9">
         <v>50</v>
       </c>
-      <c r="I16" s="16">
+      <c r="I16" s="9">
         <v>32</v>
       </c>
-      <c r="J16" s="21">
+      <c r="J16" s="18">
         <v>0.75</v>
       </c>
-      <c r="K16" s="22">
+      <c r="K16" s="15">
         <v>0.68049740791320801</v>
       </c>
-      <c r="L16" s="21">
+      <c r="L16" s="18">
         <v>0.69840000000000002</v>
       </c>
-      <c r="M16" s="22">
+      <c r="M16" s="15">
         <v>0.85450000000000004</v>
       </c>
-      <c r="N16" s="16">
+      <c r="N16" s="9">
         <v>60</v>
       </c>
-      <c r="O16" s="29" t="s">
+      <c r="O16" s="24" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="17" spans="1:15" ht="189.5" thickTop="1" thickBot="1">
-      <c r="A17" s="10"/>
-      <c r="B17" s="13">
+      <c r="A17" s="27"/>
+      <c r="B17" s="11">
         <v>4</v>
       </c>
-      <c r="C17" s="13" t="s">
+      <c r="C17" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="D17" s="13" t="s">
+      <c r="D17" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="E17" s="13">
+      <c r="E17" s="11">
         <v>20</v>
       </c>
-      <c r="F17" s="13" t="s">
+      <c r="F17" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G17" s="13">
+      <c r="G17" s="11">
         <v>1E-3</v>
       </c>
-      <c r="H17" s="14">
+      <c r="H17" s="12">
         <v>30</v>
       </c>
-      <c r="I17" s="13">
+      <c r="I17" s="11">
         <v>32</v>
       </c>
-      <c r="J17" s="19">
+      <c r="J17" s="16">
         <v>0.875</v>
       </c>
-      <c r="K17" s="20">
+      <c r="K17" s="17">
         <v>0.56066429615020696</v>
       </c>
-      <c r="L17" s="19">
+      <c r="L17" s="16">
         <v>0.81330000000000002</v>
       </c>
-      <c r="M17" s="20">
+      <c r="M17" s="17">
         <v>0.66830000000000001</v>
       </c>
-      <c r="N17" s="13">
+      <c r="N17" s="11">
         <v>63</v>
       </c>
-      <c r="O17" s="29" t="s">
+      <c r="O17" s="24" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="18" spans="1:15" ht="189.5" thickTop="1" thickBot="1">
-      <c r="A18" s="10"/>
-      <c r="B18" s="16">
+      <c r="A18" s="27"/>
+      <c r="B18" s="9">
         <v>5</v>
       </c>
-      <c r="C18" s="16" t="s">
+      <c r="C18" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="D18" s="14" t="s">
+      <c r="D18" s="12" t="s">
         <v>97</v>
       </c>
-      <c r="E18" s="16">
+      <c r="E18" s="9">
         <v>20</v>
       </c>
-      <c r="F18" s="16" t="s">
+      <c r="F18" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G18" s="16">
+      <c r="G18" s="9">
         <v>1E-3</v>
       </c>
-      <c r="H18" s="16">
+      <c r="H18" s="9">
         <v>30</v>
       </c>
-      <c r="I18" s="16">
+      <c r="I18" s="9">
         <v>32</v>
       </c>
-      <c r="J18" s="21">
+      <c r="J18" s="18">
         <v>0.8125</v>
       </c>
-      <c r="K18" s="22">
+      <c r="K18" s="15">
         <v>0.85180652141571001</v>
       </c>
-      <c r="L18" s="21">
+      <c r="L18" s="18">
         <v>0.71988797187805098</v>
       </c>
-      <c r="M18" s="22">
+      <c r="M18" s="15">
         <v>0.87082278728485096</v>
       </c>
-      <c r="N18" s="16">
+      <c r="N18" s="9">
         <v>60</v>
       </c>
-      <c r="O18" s="30" t="s">
+      <c r="O18" s="25" t="s">
         <v>108</v>
       </c>
     </row>
     <row r="19" spans="1:15" ht="175" thickTop="1" thickBot="1">
-      <c r="A19" s="10" t="s">
+      <c r="A19" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="B19" s="13">
+      <c r="B19" s="11">
         <v>1</v>
       </c>
-      <c r="C19" s="13" t="s">
+      <c r="C19" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D19" s="14" t="s">
+      <c r="D19" s="12" t="s">
         <v>99</v>
       </c>
-      <c r="E19" s="13">
+      <c r="E19" s="11">
         <v>16</v>
       </c>
-      <c r="F19" s="14" t="s">
+      <c r="F19" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="G19" s="13">
+      <c r="G19" s="11">
         <v>1E-3</v>
       </c>
-      <c r="H19" s="13">
+      <c r="H19" s="11">
         <v>30</v>
       </c>
-      <c r="I19" s="13">
+      <c r="I19" s="11">
         <v>32</v>
       </c>
-      <c r="J19" s="19">
+      <c r="J19" s="16">
         <v>0.875</v>
       </c>
-      <c r="K19" s="20">
+      <c r="K19" s="17">
         <v>0.42399662733077997</v>
       </c>
-      <c r="L19" s="19">
+      <c r="L19" s="16">
         <v>0.92349999999999999</v>
       </c>
-      <c r="M19" s="20">
+      <c r="M19" s="17">
         <v>0.3039</v>
       </c>
-      <c r="N19" s="13">
+      <c r="N19" s="11">
         <v>60</v>
       </c>
-      <c r="O19" s="15" t="s">
+      <c r="O19" s="13" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:15" ht="175" thickTop="1" thickBot="1">
-      <c r="A20" s="10"/>
-      <c r="B20" s="16">
+      <c r="A20" s="27"/>
+      <c r="B20" s="9">
         <v>2</v>
       </c>
-      <c r="C20" s="16" t="s">
+      <c r="C20" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="D20" s="14" t="s">
+      <c r="D20" s="12" t="s">
         <v>100</v>
       </c>
-      <c r="E20" s="16">
+      <c r="E20" s="9">
         <v>16</v>
       </c>
-      <c r="F20" s="16" t="s">
+      <c r="F20" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="G20" s="16">
+      <c r="G20" s="9">
         <v>1E-3</v>
       </c>
-      <c r="H20" s="16">
+      <c r="H20" s="9">
         <v>30</v>
       </c>
-      <c r="I20" s="16">
+      <c r="I20" s="9">
         <v>32</v>
       </c>
-      <c r="J20" s="21">
+      <c r="J20" s="18">
         <v>0.875</v>
       </c>
-      <c r="K20" s="22">
+      <c r="K20" s="15">
         <v>0.30894249677657998</v>
       </c>
-      <c r="L20" s="21">
+      <c r="L20" s="18">
         <v>0.98719999999999997</v>
       </c>
-      <c r="M20" s="22">
+      <c r="M20" s="15">
         <v>9.5399999999999999E-2</v>
       </c>
-      <c r="N20" s="16">
+      <c r="N20" s="9">
         <v>61</v>
       </c>
-      <c r="O20" s="24" t="s">
+      <c r="O20" s="10" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="21" spans="1:15" ht="175" thickTop="1" thickBot="1">
-      <c r="A21" s="10"/>
-      <c r="B21" s="13">
+      <c r="A21" s="27"/>
+      <c r="B21" s="11">
         <v>3</v>
       </c>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="D21" s="13" t="s">
+      <c r="D21" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="E21" s="13">
+      <c r="E21" s="11">
         <v>16</v>
       </c>
-      <c r="F21" s="13" t="s">
+      <c r="F21" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="G21" s="13">
+      <c r="G21" s="12">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="H21" s="12">
+        <v>50</v>
+      </c>
+      <c r="I21" s="11">
+        <v>32</v>
+      </c>
+      <c r="J21" s="16">
+        <v>0.875</v>
+      </c>
+      <c r="K21" s="17">
+        <v>0.51019999999999999</v>
+      </c>
+      <c r="L21" s="16">
+        <v>0.991596639156341</v>
+      </c>
+      <c r="M21" s="17">
+        <v>0.112832941114902</v>
+      </c>
+      <c r="N21" s="11">
+        <v>60</v>
+      </c>
+      <c r="O21" s="13" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15" ht="189.5" thickTop="1" thickBot="1">
+      <c r="A22" s="27"/>
+      <c r="B22" s="9">
+        <v>4</v>
+      </c>
+      <c r="C22" s="9" t="s">
+        <v>101</v>
+      </c>
+      <c r="D22" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E22" s="9">
+        <v>16</v>
+      </c>
+      <c r="F22" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="G22" s="9">
         <v>1E-3</v>
       </c>
-      <c r="H21" s="14">
+      <c r="H22" s="12">
+        <v>30</v>
+      </c>
+      <c r="I22" s="9">
+        <v>32</v>
+      </c>
+      <c r="J22" s="18">
+        <v>0.5625</v>
+      </c>
+      <c r="K22" s="15">
+        <v>1.1489222049713099</v>
+      </c>
+      <c r="L22" s="18">
+        <v>0.57422971725463801</v>
+      </c>
+      <c r="M22" s="15">
+        <v>1.11140024662017</v>
+      </c>
+      <c r="N22" s="9">
+        <v>39</v>
+      </c>
+      <c r="O22" s="10" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15" ht="189.5" thickTop="1" thickBot="1">
+      <c r="A23" s="27"/>
+      <c r="B23" s="11">
+        <v>5</v>
+      </c>
+      <c r="C23" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="E23" s="11">
+        <v>16</v>
+      </c>
+      <c r="F23" s="11" t="s">
+        <v>10</v>
+      </c>
+      <c r="G23" s="12">
+        <v>5.0000000000000001E-4</v>
+      </c>
+      <c r="H23" s="12">
         <v>50</v>
       </c>
-      <c r="I21" s="13">
+      <c r="I23" s="11">
         <v>32</v>
       </c>
-      <c r="J21" s="19">
-        <v>0.87</v>
-      </c>
-      <c r="K21" s="20">
-        <v>0.480497407913208</v>
-      </c>
-      <c r="L21" s="19">
-        <v>0.96840000000000004</v>
-      </c>
-      <c r="M21" s="20">
-        <v>0.35449999999999998</v>
-      </c>
-      <c r="N21" s="13">
-        <v>60</v>
-      </c>
-      <c r="O21" s="15" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="22" spans="1:15" ht="189.5" thickTop="1" thickBot="1">
-      <c r="A22" s="10"/>
-      <c r="B22" s="16">
-        <v>4</v>
-      </c>
-      <c r="C22" s="16" t="s">
+      <c r="J23" s="16">
+        <v>0.625</v>
+      </c>
+      <c r="K23" s="17">
+        <v>0.96765786409377996</v>
+      </c>
+      <c r="L23" s="16">
+        <v>0.680672287940979</v>
+      </c>
+      <c r="M23" s="17">
+        <v>0.85677433013916005</v>
+      </c>
+      <c r="N23" s="11">
+        <v>46</v>
+      </c>
+      <c r="O23" s="24" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15" ht="247.5" thickTop="1" thickBot="1">
+      <c r="A24" s="19"/>
+      <c r="B24" s="20">
+        <v>6</v>
+      </c>
+      <c r="C24" s="20" t="s">
         <v>101</v>
       </c>
-      <c r="D22" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="E22" s="16">
+      <c r="D24" s="21" t="s">
+        <v>103</v>
+      </c>
+      <c r="E24" s="20">
         <v>16</v>
       </c>
-      <c r="F22" s="16" t="s">
+      <c r="F24" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="G22" s="16">
+      <c r="G24" s="21">
         <v>1E-3</v>
       </c>
-      <c r="H22" s="14">
+      <c r="H24" s="21">
         <v>30</v>
       </c>
-      <c r="I22" s="16">
+      <c r="I24" s="20">
         <v>32</v>
       </c>
-      <c r="J22" s="21">
-        <v>0.5625</v>
-      </c>
-      <c r="K22" s="22">
-        <v>1.1489222049713099</v>
-      </c>
-      <c r="L22" s="21">
-        <v>0.57422971725463801</v>
-      </c>
-      <c r="M22" s="22">
-        <v>1.11140024662017</v>
-      </c>
-      <c r="N22" s="16">
-        <v>39</v>
-      </c>
-      <c r="O22" s="24" t="s">
-        <v>111</v>
-      </c>
-    </row>
-    <row r="23" spans="1:15" ht="189.5" thickTop="1" thickBot="1">
-      <c r="A23" s="10"/>
-      <c r="B23" s="13">
-        <v>5</v>
-      </c>
-      <c r="C23" s="13" t="s">
-        <v>101</v>
-      </c>
-      <c r="D23" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="E23" s="13">
-        <v>16</v>
-      </c>
-      <c r="F23" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="G23" s="14">
-        <v>5.0000000000000001E-4</v>
-      </c>
-      <c r="H23" s="14">
-        <v>50</v>
-      </c>
-      <c r="I23" s="13">
-        <v>32</v>
-      </c>
-      <c r="J23" s="19">
-        <v>0.625</v>
-      </c>
-      <c r="K23" s="20">
-        <v>0.96765786409377996</v>
-      </c>
-      <c r="L23" s="19">
-        <v>0.680672287940979</v>
-      </c>
-      <c r="M23" s="20">
-        <v>0.85677433013916005</v>
-      </c>
-      <c r="N23" s="13">
-        <v>46</v>
-      </c>
-      <c r="O23" s="29" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="24" spans="1:15" ht="247.5" thickTop="1" thickBot="1">
-      <c r="A24" s="23"/>
-      <c r="B24" s="25">
-        <v>6</v>
-      </c>
-      <c r="C24" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="D24" s="26" t="s">
-        <v>103</v>
-      </c>
-      <c r="E24" s="25">
-        <v>16</v>
-      </c>
-      <c r="F24" s="25" t="s">
-        <v>10</v>
-      </c>
-      <c r="G24" s="26">
-        <v>1E-3</v>
-      </c>
-      <c r="H24" s="26">
-        <v>30</v>
-      </c>
-      <c r="I24" s="25">
-        <v>32</v>
-      </c>
-      <c r="J24" s="27">
+      <c r="J24" s="22">
         <v>0.875</v>
       </c>
-      <c r="K24" s="28">
+      <c r="K24" s="23">
         <v>0.212697088718414</v>
       </c>
-      <c r="L24" s="27">
+      <c r="L24" s="22">
         <v>0.96009999999999995</v>
       </c>
-      <c r="M24" s="28">
+      <c r="M24" s="23">
         <v>0.1241</v>
       </c>
-      <c r="N24" s="25">
+      <c r="N24" s="20">
         <v>48</v>
       </c>
-      <c r="O24" s="31" t="s">
+      <c r="O24" s="26" t="s">
         <v>113</v>
       </c>
     </row>
@@ -2138,7 +2129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{690A8F4C-0D72-42AE-9F5C-0C5E934BF194}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -2177,7 +2168,7 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="28" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
@@ -2203,7 +2194,7 @@
       </c>
     </row>
     <row r="3" spans="1:9">
-      <c r="A3" s="5"/>
+      <c r="A3" s="28"/>
       <c r="B3" s="1" t="s">
         <v>22</v>
       </c>
@@ -2227,7 +2218,7 @@
       </c>
     </row>
     <row r="4" spans="1:9">
-      <c r="A4" s="5"/>
+      <c r="A4" s="28"/>
       <c r="B4" s="1" t="s">
         <v>24</v>
       </c>
@@ -2251,7 +2242,7 @@
       </c>
     </row>
     <row r="5" spans="1:9">
-      <c r="A5" s="5"/>
+      <c r="A5" s="28"/>
       <c r="B5" s="1" t="s">
         <v>26</v>
       </c>
@@ -2275,7 +2266,7 @@
       </c>
     </row>
     <row r="6" spans="1:9">
-      <c r="A6" s="5"/>
+      <c r="A6" s="28"/>
       <c r="B6" s="1" t="s">
         <v>28</v>
       </c>
@@ -2299,7 +2290,7 @@
       </c>
     </row>
     <row r="7" spans="1:9">
-      <c r="A7" s="5"/>
+      <c r="A7" s="28"/>
       <c r="B7" s="1" t="s">
         <v>30</v>
       </c>
@@ -2323,7 +2314,7 @@
       </c>
     </row>
     <row r="8" spans="1:9">
-      <c r="A8" s="5"/>
+      <c r="A8" s="28"/>
       <c r="B8" s="1" t="s">
         <v>32</v>
       </c>
@@ -2347,7 +2338,7 @@
       </c>
     </row>
     <row r="9" spans="1:9">
-      <c r="A9" s="5"/>
+      <c r="A9" s="28"/>
       <c r="B9" s="1" t="s">
         <v>34</v>
       </c>
@@ -2371,7 +2362,7 @@
       </c>
     </row>
     <row r="10" spans="1:9">
-      <c r="A10" s="5"/>
+      <c r="A10" s="28"/>
       <c r="B10" s="1" t="s">
         <v>36</v>
       </c>
@@ -2395,7 +2386,7 @@
       </c>
     </row>
     <row r="11" spans="1:9">
-      <c r="A11" s="5"/>
+      <c r="A11" s="28"/>
       <c r="B11" s="1" t="s">
         <v>38</v>
       </c>
@@ -2419,7 +2410,7 @@
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="5"/>
+      <c r="A12" s="28"/>
       <c r="B12" s="1" t="s">
         <v>40</v>
       </c>
@@ -2443,7 +2434,7 @@
       </c>
     </row>
     <row r="13" spans="1:9">
-      <c r="A13" s="5"/>
+      <c r="A13" s="28"/>
       <c r="B13" s="1" t="s">
         <v>42</v>
       </c>
@@ -2467,7 +2458,7 @@
       </c>
     </row>
     <row r="14" spans="1:9">
-      <c r="A14" s="5" t="s">
+      <c r="A14" s="28" t="s">
         <v>11</v>
       </c>
       <c r="B14" s="1" t="s">
@@ -2493,7 +2484,7 @@
       </c>
     </row>
     <row r="15" spans="1:9">
-      <c r="A15" s="5"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="1" t="s">
         <v>46</v>
       </c>
@@ -2517,7 +2508,7 @@
       </c>
     </row>
     <row r="16" spans="1:9">
-      <c r="A16" s="5"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="1" t="s">
         <v>48</v>
       </c>
@@ -2541,7 +2532,7 @@
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="5"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="1" t="s">
         <v>50</v>
       </c>
@@ -2565,7 +2556,7 @@
       </c>
     </row>
     <row r="18" spans="1:9">
-      <c r="A18" s="5"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="1" t="s">
         <v>52</v>
       </c>
@@ -2589,7 +2580,7 @@
       </c>
     </row>
     <row r="19" spans="1:9">
-      <c r="A19" s="5" t="s">
+      <c r="A19" s="28" t="s">
         <v>12</v>
       </c>
       <c r="B19" s="1" t="s">
@@ -2615,7 +2606,7 @@
       </c>
     </row>
     <row r="20" spans="1:9">
-      <c r="A20" s="5"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="1" t="s">
         <v>56</v>
       </c>
@@ -2639,7 +2630,7 @@
       </c>
     </row>
     <row r="21" spans="1:9">
-      <c r="A21" s="5"/>
+      <c r="A21" s="28"/>
       <c r="B21" s="1" t="s">
         <v>58</v>
       </c>
@@ -2663,7 +2654,7 @@
       </c>
     </row>
     <row r="22" spans="1:9">
-      <c r="A22" s="5"/>
+      <c r="A22" s="28"/>
       <c r="B22" s="1" t="s">
         <v>60</v>
       </c>
@@ -2687,7 +2678,7 @@
       </c>
     </row>
     <row r="23" spans="1:9">
-      <c r="A23" s="5"/>
+      <c r="A23" s="28"/>
       <c r="B23" s="1" t="s">
         <v>70</v>
       </c>

</xml_diff>

<commit_message>
Conclusion and final recommendation added in Notebook
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Arnab Learning\AI_ML_DS\EPGP_IIITB_Upgrad\Course 7 - Course 4 - Deep Learning\Module 7 - Gesture Recognition Project\Git_Repo\Gesture-Recognition-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AD6B1C-A2BB-457E-8DE5-7C8B91EC88AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{235570A8-D65B-456A-81F7-72F1C4479F4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{5F067AC9-599E-4E59-A365-A6D113994EE3}"/>
   </bookViews>
@@ -1016,7 +1016,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80923883-5B62-4AF5-AE7C-62BC6F87EDBB}">
   <dimension ref="A1:O24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="T24" sqref="T24"/>
     </sheetView>
   </sheetViews>
@@ -2129,7 +2129,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{690A8F4C-0D72-42AE-9F5C-0C5E934BF194}">
   <dimension ref="A1:I24"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="A7" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>